<commit_message>
direct matching between acts and risk points
</commit_message>
<xml_diff>
--- a/source/작업행동.xlsx
+++ b/source/작업행동.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my_develop\matching\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8957D332-366C-4C74-AB77-F0D771A8BDCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448688E0-9CBA-4982-A98A-7B2D8A67F9F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-45" yWindow="525" windowWidth="12615" windowHeight="5460" xr2:uid="{7DE75812-C78E-412C-9C8F-3FB0D22FA83F}"/>
+    <workbookView xWindow="495" yWindow="0" windowWidth="12615" windowHeight="15450" xr2:uid="{7DE75812-C78E-412C-9C8F-3FB0D22FA83F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -312,9 +312,6 @@
   </si>
   <si>
     <t>행_30</t>
-  </si>
-  <si>
-    <t>행_31</t>
   </si>
 </sst>
 </file>
@@ -687,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40BEB60D-F08D-4AA7-B205-DF61B0E4BD78}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -752,17 +749,22 @@
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -770,10 +772,10 @@
         <v>67</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -781,10 +783,10 @@
         <v>68</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -792,10 +794,10 @@
         <v>69</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -803,10 +805,10 @@
         <v>70</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -814,21 +816,21 @@
         <v>71</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>27</v>
+      <c r="B12" t="s">
+        <v>29</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -836,10 +838,10 @@
         <v>73</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -847,10 +849,10 @@
         <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -858,10 +860,10 @@
         <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -869,10 +871,10 @@
         <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -880,10 +882,10 @@
         <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -891,10 +893,10 @@
         <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -902,10 +904,10 @@
         <v>79</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -913,10 +915,10 @@
         <v>80</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -924,10 +926,10 @@
         <v>81</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -935,10 +937,10 @@
         <v>82</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -946,10 +948,10 @@
         <v>83</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -957,10 +959,10 @@
         <v>84</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -968,10 +970,10 @@
         <v>85</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -979,10 +981,10 @@
         <v>86</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -990,10 +992,10 @@
         <v>87</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -1001,10 +1003,10 @@
         <v>88</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1012,10 +1014,10 @@
         <v>89</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -1023,10 +1025,10 @@
         <v>90</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1034,20 +1036,9 @@
         <v>91</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B32" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" s="2" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>